<commit_message>
manipulation on gis file
</commit_message>
<xml_diff>
--- a/data/data_from_M/Site Characteristics for Capstone Students.xlsx
+++ b/data/data_from_M/Site Characteristics for Capstone Students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaosiyue/Documents/Columbia MSPH/Spring 2023/P9300 - Capstone/ehs_capstone_nycdoh/data/data_from_M/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C7433A-A187-5140-9C3D-D54927C8B438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2B03CC-54B8-754C-B157-D5C53CB6B760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{DD4B28C4-0AF3-4A41-BCD1-E3D14D8E4613}"/>
   </bookViews>
@@ -7412,7 +7412,7 @@
     <t>12CBCP019K</t>
   </si>
   <si>
-    <t>11CBCP015K</t>
+    <t>11CVCP015K</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
correct an error for the dfs
</commit_message>
<xml_diff>
--- a/data/data_from_M/Site Characteristics for Capstone Students.xlsx
+++ b/data/data_from_M/Site Characteristics for Capstone Students.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaosiyue/Documents/Columbia MSPH/Spring 2023/P9300 - Capstone/ehs_capstone_nycdoh/data/data_from_M/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2B03CC-54B8-754C-B157-D5C53CB6B760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0458AB4-B66A-6F4C-B690-50F6F00A42AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{DD4B28C4-0AF3-4A41-BCD1-E3D14D8E4613}"/>
+    <workbookView xWindow="-2160" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{DD4B28C4-0AF3-4A41-BCD1-E3D14D8E4613}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7813,8 +7813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624F314B-8255-4B45-8931-CE0A92D26BCE}">
   <dimension ref="A1:X443"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A413" workbookViewId="0">
+      <selection activeCell="F442" sqref="F442"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40471,7 +40471,7 @@
         <v>21</v>
       </c>
       <c r="F442" s="1">
-        <v>11214</v>
+        <v>11232</v>
       </c>
       <c r="G442" s="1">
         <v>985414</v>

</xml_diff>